<commit_message>
add more to files
</commit_message>
<xml_diff>
--- a/initial_data/initial_data.xlsx
+++ b/initial_data/initial_data.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9528" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="category" sheetId="1" r:id="rId1"/>
     <sheet name="products" sheetId="2" r:id="rId2"/>
+    <sheet name="purchase" sheetId="3" r:id="rId3"/>
+    <sheet name="customers" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Category</t>
   </si>
@@ -127,6 +129,39 @@
   </si>
   <si>
     <t>Blouse</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>customerkey</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>Ebuka</t>
+  </si>
+  <si>
+    <t>Ifechukwu</t>
+  </si>
+  <si>
+    <t>Chidera</t>
+  </si>
+  <si>
+    <t>Ugonna</t>
+  </si>
+  <si>
+    <t>Uchenna</t>
   </si>
 </sst>
 </file>
@@ -497,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -955,4 +990,110 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>LEFT(B2,3)&amp;LEFT(C2,3)</f>
+        <v>EbuIfe</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A5" si="0">LEFT(B3,3)&amp;LEFT(C3,3)</f>
+        <v>ChiIfe</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>UgoIfe</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>UchIfe</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
connect db_interact to user_interact
</commit_message>
<xml_diff>
--- a/initial_data/initial_data.xlsx
+++ b/initial_data/initial_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\store_management\initial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E2F902-D009-4B0C-9508-48F5CA947A1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9528" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="category" sheetId="1" r:id="rId1"/>
@@ -17,17 +18,22 @@
     <sheet name="purchase" sheetId="3" r:id="rId3"/>
     <sheet name="customers" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Category</t>
   </si>
@@ -162,12 +168,15 @@
   </si>
   <si>
     <t>Uchenna</t>
+  </si>
+  <si>
+    <t>pk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -478,7 +487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -529,17 +538,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" customWidth="1"/>
     <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" customWidth="1"/>
@@ -993,16 +1002,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1014,6 +1026,9 @@
       </c>
       <c r="D1" t="s">
         <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1022,11 +1037,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>